<commit_message>
& - №71214195 от 28.09.2024 https://meshok.net/ - №71214242 от 28.09.2024 https://meshok.net/
</commit_message>
<xml_diff>
--- a/Collections/USA/#USA#Commemorative#[1999-present]#circulation_quality.xlsx
+++ b/Collections/USA/#USA#Commemorative#[1999-present]#circulation_quality.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lord_Alexator\Documents\CoinCollection\Collections\USA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51DE8B6E-9790-4DC1-855B-E13F4AAFF6A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91CCDF54-902B-4DF2-9650-5E936E293DC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" firstSheet="3" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4910" yWindow="630" windowWidth="28720" windowHeight="19550" firstSheet="3" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="&quot;Linkoln_Cents&quot;" sheetId="7" r:id="rId1"/>
@@ -9433,11 +9433,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1FB08FCB-4607-4875-B1CE-F05341C08ADF}">
   <dimension ref="A1:K23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="11" ySplit="2" topLeftCell="L3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="L1" sqref="L1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="K21" sqref="K21"/>
+      <selection pane="bottomRight" activeCell="K18" sqref="K18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -10048,7 +10048,7 @@
       <selection activeCell="C15" sqref="C15"/>
       <selection pane="topRight" activeCell="C15" sqref="C15"/>
       <selection pane="bottomLeft" activeCell="C15" sqref="C15"/>
-      <selection pane="bottomRight" activeCell="B41" sqref="B38:H41"/>
+      <selection pane="bottomRight" activeCell="J26" sqref="J26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -10427,7 +10427,7 @@
         <v>5</v>
       </c>
       <c r="H13" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I13" s="9" t="str">
         <f t="shared" si="0"/>
@@ -10484,7 +10484,7 @@
         <v>392</v>
       </c>
       <c r="G15" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H15" s="1">
         <v>1</v>
@@ -10514,10 +10514,10 @@
         <v>395</v>
       </c>
       <c r="G16" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H16" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I16" s="9" t="str">
         <f t="shared" si="0"/>
@@ -10544,7 +10544,7 @@
         <v>398</v>
       </c>
       <c r="G17" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H17" s="1">
         <v>1</v>
@@ -10814,14 +10814,14 @@
         <v>420</v>
       </c>
       <c r="G26" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H26" s="1">
         <v>0</v>
       </c>
       <c r="I26" s="9" t="str">
         <f t="shared" si="0"/>
-        <v/>
+        <v>Can exchange</v>
       </c>
     </row>
     <row r="27" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
@@ -10994,7 +10994,7 @@
         <v>432</v>
       </c>
       <c r="G32" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H32" s="1">
         <v>1</v>
@@ -11174,7 +11174,7 @@
         <v>418</v>
       </c>
       <c r="G38" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H38" s="1">
         <v>1</v>
@@ -11356,12 +11356,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:I28"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="8" ySplit="2" topLeftCell="I3" activePane="bottomRight" state="frozen"/>
       <selection activeCell="C15" sqref="C15"/>
       <selection pane="topRight" activeCell="C15" sqref="C15"/>
       <selection pane="bottomLeft" activeCell="C15" sqref="C15"/>
-      <selection pane="bottomRight" activeCell="H25" sqref="H25"/>
+      <selection pane="bottomRight" activeCell="I23" sqref="I23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -11439,7 +11439,7 @@
         <v>3</v>
       </c>
       <c r="H3" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I3" s="9" t="str">
         <f t="shared" ref="I3:I22" si="0">IF(OR(AND(G3&gt;1,G3&lt;&gt;"-"),AND(H3&gt;1,H3&lt;&gt;"-")),"Can exchange","")</f>
@@ -11467,7 +11467,7 @@
         <v>0</v>
       </c>
       <c r="H4" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I4" s="9" t="str">
         <f t="shared" si="0"/>
@@ -11495,7 +11495,7 @@
         <v>0</v>
       </c>
       <c r="H5" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I5" s="9" t="str">
         <f t="shared" si="0"/>
@@ -11523,7 +11523,7 @@
         <v>0</v>
       </c>
       <c r="H6" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I6" s="9" t="str">
         <f t="shared" si="0"/>
@@ -11551,7 +11551,7 @@
         <v>0</v>
       </c>
       <c r="H7" s="53">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I7" s="9" t="str">
         <f t="shared" si="0"/>
@@ -11579,7 +11579,7 @@
         <v>0</v>
       </c>
       <c r="H8" s="58">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I8" s="9" t="str">
         <f t="shared" si="0"/>
@@ -11607,7 +11607,7 @@
         <v>0</v>
       </c>
       <c r="H9" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I9" s="9" t="str">
         <f t="shared" si="0"/>
@@ -11635,7 +11635,7 @@
         <v>0</v>
       </c>
       <c r="H10" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I10" s="9" t="str">
         <f t="shared" si="0"/>
@@ -11663,7 +11663,7 @@
         <v>0</v>
       </c>
       <c r="H11" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I11" s="9" t="str">
         <f t="shared" si="0"/>
@@ -11691,7 +11691,7 @@
         <v>1</v>
       </c>
       <c r="H12" s="53">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I12" s="9" t="str">
         <f t="shared" si="0"/>
@@ -11744,10 +11744,10 @@
         <v>6</v>
       </c>
       <c r="G14" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H14" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I14" s="9" t="str">
         <f t="shared" si="0"/>
@@ -11772,10 +11772,10 @@
         <v>8</v>
       </c>
       <c r="G15" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H15" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I15" s="9" t="str">
         <f t="shared" si="0"/>
@@ -11800,7 +11800,7 @@
         <v>9</v>
       </c>
       <c r="G16" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H16" s="1">
         <v>1</v>
@@ -11831,7 +11831,7 @@
         <v>1</v>
       </c>
       <c r="H17" s="53">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I17" s="9" t="str">
         <f t="shared" si="0"/>
@@ -11859,7 +11859,7 @@
         <v>1</v>
       </c>
       <c r="H18" s="58">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I18" s="9" t="str">
         <f t="shared" si="0"/>
@@ -11887,7 +11887,7 @@
         <v>1</v>
       </c>
       <c r="H19" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I19" s="9" t="str">
         <f t="shared" si="0"/>

</xml_diff>

<commit_message>
& - №71297326 от 01.10.2024 https://meshok.net/
</commit_message>
<xml_diff>
--- a/Collections/USA/#USA#Commemorative#[1999-present]#circulation_quality.xlsx
+++ b/Collections/USA/#USA#Commemorative#[1999-present]#circulation_quality.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lord_Alexator\Documents\CoinCollection\Collections\USA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F41F0C23-3DCE-42E3-9A87-031533D4D3F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0EA13A1-2358-45BD-9CBE-6F4A41139BA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" firstSheet="1" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9680" yWindow="1450" windowWidth="28720" windowHeight="19550" firstSheet="3" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="&quot;Linkoln_Cents&quot;" sheetId="7" r:id="rId1"/>
@@ -832,6 +832,7 @@
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Пользователь Windows</author>
+    <author>Lord_Alexator</author>
   </authors>
   <commentList>
     <comment ref="E2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-000001000000}">
@@ -912,6 +913,21 @@
             <charset val="204"/>
           </rPr>
           <t xml:space="preserve">
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G3" authorId="1" shapeId="0" xr:uid="{BAB4F641-BADD-4C8F-AD39-B9B12F23FFAB}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="204"/>
+          </rPr>
+          <t xml:space="preserve">Дубли не UNC
 </t>
         </r>
       </text>
@@ -3167,7 +3183,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -3254,6 +3270,13 @@
       <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
       <charset val="204"/>
     </font>
   </fonts>
@@ -3573,7 +3596,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="102">
+  <cellXfs count="104">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -3858,12 +3881,26 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Гиперссылка" xfId="1" builtinId="8"/>
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="55">
+  <dxfs count="56">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF9BE5FF"/>
+          <bgColor rgb="FF9BE5FF"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -4310,9 +4347,9 @@
     <filterColumn colId="2" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="№" dataDxfId="2"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Link" dataDxfId="1" dataCellStyle="Гиперссылка"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Description (single table, table set, mintage, prices):" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="№" dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Link" dataDxfId="2" dataCellStyle="Гиперссылка"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Description (single table, table set, mintage, prices):" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="1" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
@@ -4830,7 +4867,7 @@
     <mergeCell ref="H1:J1"/>
   </mergeCells>
   <conditionalFormatting sqref="H3:J5">
-    <cfRule type="containsText" dxfId="54" priority="7" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="55" priority="7" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(H3))))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4847,7 +4884,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J6">
-    <cfRule type="containsText" dxfId="53" priority="5" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="54" priority="5" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(J6))))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4864,7 +4901,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H6">
-    <cfRule type="containsText" dxfId="52" priority="3" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="53" priority="3" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(H6))))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4881,7 +4918,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I6">
-    <cfRule type="containsText" dxfId="51" priority="1" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="52" priority="1" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(I6))))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5125,7 +5162,7 @@
     <mergeCell ref="H1:J1"/>
   </mergeCells>
   <conditionalFormatting sqref="H3:J6">
-    <cfRule type="containsText" dxfId="50" priority="1" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="51" priority="1" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(H3))))</formula>
     </cfRule>
     <cfRule type="colorScale" priority="2">
@@ -6793,7 +6830,7 @@
     <mergeCell ref="C1:D1"/>
   </mergeCells>
   <conditionalFormatting sqref="G3:H58">
-    <cfRule type="containsText" dxfId="49" priority="4" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="50" priority="4" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(G3))))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -9288,7 +9325,7 @@
   </mergeCells>
   <phoneticPr fontId="12" type="noConversion"/>
   <conditionalFormatting sqref="I3:J12 L48 L50:L51 I13:K58">
-    <cfRule type="containsText" dxfId="48" priority="18" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="49" priority="18" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(I3))))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -9305,7 +9342,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K3:K7">
-    <cfRule type="containsText" dxfId="47" priority="13" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="48" priority="13" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(K3))))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -9322,7 +9359,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K8:K12">
-    <cfRule type="containsText" dxfId="46" priority="11" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="47" priority="11" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(K8))))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -9339,12 +9376,12 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L8:L47">
-    <cfRule type="containsText" dxfId="45" priority="5" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="46" priority="5" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(L8))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L52:L57">
-    <cfRule type="containsText" dxfId="44" priority="9" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="45" priority="9" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(L52))))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -9361,7 +9398,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L3:L7">
-    <cfRule type="containsText" dxfId="43" priority="7" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="44" priority="7" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(L3))))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -9390,7 +9427,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L49">
-    <cfRule type="containsText" dxfId="42" priority="3" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="43" priority="3" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(L49))))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -9407,7 +9444,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L58">
-    <cfRule type="containsText" dxfId="41" priority="1" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="42" priority="1" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(L58))))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -10000,7 +10037,7 @@
   </mergeCells>
   <phoneticPr fontId="12" type="noConversion"/>
   <conditionalFormatting sqref="H3:I17">
-    <cfRule type="containsText" dxfId="40" priority="15" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="41" priority="15" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(H3))))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -10017,7 +10054,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J3:J17">
-    <cfRule type="containsText" dxfId="39" priority="1" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="40" priority="1" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(J3))))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -10048,7 +10085,7 @@
       <selection activeCell="C15" sqref="C15"/>
       <selection pane="topRight" activeCell="C15" sqref="C15"/>
       <selection pane="bottomLeft" activeCell="C15" sqref="C15"/>
-      <selection pane="bottomRight" activeCell="J38" sqref="J38"/>
+      <selection pane="bottomRight" activeCell="I27" sqref="I27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -11313,7 +11350,7 @@
     <mergeCell ref="E1:F1"/>
   </mergeCells>
   <conditionalFormatting sqref="G3:H41">
-    <cfRule type="containsText" dxfId="38" priority="6" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="39" priority="6" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(G3))))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -11330,7 +11367,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G42:H42">
-    <cfRule type="containsText" dxfId="37" priority="1" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="38" priority="1" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(G42))))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -11361,7 +11398,7 @@
       <selection activeCell="C15" sqref="C15"/>
       <selection pane="topRight" activeCell="C15" sqref="C15"/>
       <selection pane="bottomLeft" activeCell="C15" sqref="C15"/>
-      <selection pane="bottomRight" activeCell="L36" sqref="L36"/>
+      <selection pane="bottomRight" activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -11435,8 +11472,8 @@
       <c r="F3" s="5" t="s">
         <v>496</v>
       </c>
-      <c r="G3" s="1">
-        <v>3</v>
+      <c r="G3" s="102">
+        <v>4</v>
       </c>
       <c r="H3" s="1">
         <v>1</v>
@@ -11464,7 +11501,7 @@
         <v>498</v>
       </c>
       <c r="G4" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H4" s="1">
         <v>1</v>
@@ -11492,7 +11529,7 @@
         <v>500</v>
       </c>
       <c r="G5" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H5" s="1">
         <v>1</v>
@@ -11520,7 +11557,7 @@
         <v>8</v>
       </c>
       <c r="G6" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H6" s="1">
         <v>1</v>
@@ -11548,7 +11585,7 @@
         <v>501</v>
       </c>
       <c r="G7" s="53">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H7" s="53">
         <v>1</v>
@@ -11576,7 +11613,7 @@
         <v>502</v>
       </c>
       <c r="G8" s="58">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H8" s="58">
         <v>1</v>
@@ -11604,7 +11641,7 @@
         <v>7</v>
       </c>
       <c r="G9" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H9" s="1">
         <v>1</v>
@@ -11632,7 +11669,7 @@
         <v>420</v>
       </c>
       <c r="G10" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H10" s="1">
         <v>1</v>
@@ -11660,7 +11697,7 @@
         <v>9</v>
       </c>
       <c r="G11" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H11" s="1">
         <v>1</v>
@@ -11687,7 +11724,7 @@
       <c r="F12" s="52" t="s">
         <v>2</v>
       </c>
-      <c r="G12" s="53">
+      <c r="G12" s="103">
         <v>1</v>
       </c>
       <c r="H12" s="53">
@@ -12124,12 +12161,12 @@
     <mergeCell ref="C1:D1"/>
   </mergeCells>
   <conditionalFormatting sqref="G12:H22">
-    <cfRule type="containsText" dxfId="36" priority="56" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="37" priority="58" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(G12))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G12:H22">
-    <cfRule type="colorScale" priority="57">
+    <cfRule type="colorScale" priority="59">
       <colorScale>
         <cfvo type="formula" val="0"/>
         <cfvo type="formula" val="1"/>
@@ -12141,22 +12178,22 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G12:H22">
-    <cfRule type="cellIs" dxfId="35" priority="58" operator="equal">
+    <cfRule type="cellIs" dxfId="36" priority="60" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G12:H22">
-    <cfRule type="cellIs" dxfId="34" priority="59" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="35" priority="61" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G3:H11">
-    <cfRule type="containsText" dxfId="33" priority="49" operator="containsText" text="*-">
+  <conditionalFormatting sqref="G4:H11 H3">
+    <cfRule type="containsText" dxfId="34" priority="51" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(G3))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G3:H11">
-    <cfRule type="colorScale" priority="50">
+  <conditionalFormatting sqref="G4:H11 H3">
+    <cfRule type="colorScale" priority="52">
       <colorScale>
         <cfvo type="formula" val="0"/>
         <cfvo type="formula" val="1"/>
@@ -12167,23 +12204,23 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G3:H11">
-    <cfRule type="cellIs" dxfId="32" priority="51" operator="equal">
+  <conditionalFormatting sqref="G4:H11 H3">
+    <cfRule type="cellIs" dxfId="33" priority="53" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G3:H11">
-    <cfRule type="cellIs" dxfId="31" priority="52" operator="greaterThan">
+  <conditionalFormatting sqref="G4:H11 H3">
+    <cfRule type="cellIs" dxfId="32" priority="54" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G23:H23">
-    <cfRule type="containsText" dxfId="30" priority="45" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="31" priority="47" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(G23))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G23:H23">
-    <cfRule type="colorScale" priority="46">
+    <cfRule type="colorScale" priority="48">
       <colorScale>
         <cfvo type="formula" val="0"/>
         <cfvo type="formula" val="1"/>
@@ -12195,22 +12232,22 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G23:H23">
-    <cfRule type="cellIs" dxfId="29" priority="47" operator="equal">
+    <cfRule type="cellIs" dxfId="30" priority="49" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G23:H23">
-    <cfRule type="cellIs" dxfId="28" priority="48" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="29" priority="50" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G24">
-    <cfRule type="containsText" dxfId="27" priority="37" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="28" priority="39" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(G24))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G24">
-    <cfRule type="colorScale" priority="38">
+    <cfRule type="colorScale" priority="40">
       <colorScale>
         <cfvo type="formula" val="0"/>
         <cfvo type="formula" val="1"/>
@@ -12222,22 +12259,22 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G24">
-    <cfRule type="cellIs" dxfId="26" priority="39" operator="equal">
+    <cfRule type="cellIs" dxfId="27" priority="41" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G24">
-    <cfRule type="cellIs" dxfId="25" priority="40" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="26" priority="42" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H24">
-    <cfRule type="containsText" dxfId="24" priority="33" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="25" priority="35" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(H24))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H24">
-    <cfRule type="colorScale" priority="34">
+    <cfRule type="colorScale" priority="36">
       <colorScale>
         <cfvo type="formula" val="0"/>
         <cfvo type="formula" val="1"/>
@@ -12249,22 +12286,22 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H24">
-    <cfRule type="cellIs" dxfId="23" priority="35" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="37" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H24">
-    <cfRule type="cellIs" dxfId="22" priority="36" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="23" priority="38" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G25">
-    <cfRule type="containsText" dxfId="21" priority="29" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="22" priority="31" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(G25))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G25">
-    <cfRule type="colorScale" priority="30">
+    <cfRule type="colorScale" priority="32">
       <colorScale>
         <cfvo type="formula" val="0"/>
         <cfvo type="formula" val="1"/>
@@ -12276,22 +12313,22 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G25">
-    <cfRule type="cellIs" dxfId="20" priority="31" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="33" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G25">
-    <cfRule type="cellIs" dxfId="19" priority="32" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="20" priority="34" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H25">
-    <cfRule type="containsText" dxfId="18" priority="25" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="19" priority="27" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(H25))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H25">
-    <cfRule type="colorScale" priority="26">
+    <cfRule type="colorScale" priority="28">
       <colorScale>
         <cfvo type="formula" val="0"/>
         <cfvo type="formula" val="1"/>
@@ -12303,22 +12340,22 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H25">
-    <cfRule type="cellIs" dxfId="17" priority="27" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="29" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H25">
-    <cfRule type="cellIs" dxfId="16" priority="28" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="17" priority="30" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G26">
-    <cfRule type="containsText" dxfId="15" priority="21" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="16" priority="23" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(G26))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G26">
-    <cfRule type="colorScale" priority="22">
+    <cfRule type="colorScale" priority="24">
       <colorScale>
         <cfvo type="formula" val="0"/>
         <cfvo type="formula" val="1"/>
@@ -12330,22 +12367,22 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G26">
-    <cfRule type="cellIs" dxfId="14" priority="23" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="25" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G26">
-    <cfRule type="cellIs" dxfId="13" priority="24" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="14" priority="26" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H26">
-    <cfRule type="containsText" dxfId="12" priority="17" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="13" priority="19" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(H26))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H26">
-    <cfRule type="colorScale" priority="18">
+    <cfRule type="colorScale" priority="20">
       <colorScale>
         <cfvo type="formula" val="0"/>
         <cfvo type="formula" val="1"/>
@@ -12357,22 +12394,22 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H26">
-    <cfRule type="cellIs" dxfId="11" priority="19" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="21" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H26">
-    <cfRule type="cellIs" dxfId="10" priority="20" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="11" priority="22" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G27">
-    <cfRule type="containsText" dxfId="9" priority="13" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="10" priority="15" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(G27))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G27">
-    <cfRule type="colorScale" priority="14">
+    <cfRule type="colorScale" priority="16">
       <colorScale>
         <cfvo type="formula" val="0"/>
         <cfvo type="formula" val="1"/>
@@ -12384,22 +12421,22 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G27">
-    <cfRule type="cellIs" dxfId="8" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="17" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G27">
-    <cfRule type="cellIs" dxfId="7" priority="16" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="8" priority="18" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H27">
-    <cfRule type="containsText" dxfId="6" priority="9" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="7" priority="11" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(H27))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H27">
-    <cfRule type="colorScale" priority="10">
+    <cfRule type="colorScale" priority="12">
       <colorScale>
         <cfvo type="formula" val="0"/>
         <cfvo type="formula" val="1"/>
@@ -12411,13 +12448,30 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H27">
-    <cfRule type="cellIs" dxfId="5" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="13" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H27">
-    <cfRule type="cellIs" dxfId="4" priority="12" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="5" priority="14" operator="greaterThan">
       <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G3">
+    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="*-">
+      <formula>NOT(ISERROR(SEARCH(("*-"),(G3))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G3">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="formula" val="0"/>
+        <cfvo type="formula" val="1"/>
+        <cfvo type="formula" val="10"/>
+        <color rgb="FFFF9F9F"/>
+        <color rgb="FFD1E0B2"/>
+        <color rgb="FF00B050"/>
+      </colorScale>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
@@ -14001,7 +14055,7 @@
     <mergeCell ref="C1:D1"/>
   </mergeCells>
   <conditionalFormatting sqref="G3:H59">
-    <cfRule type="containsText" dxfId="3" priority="78" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="4" priority="78" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(G3))))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>